<commit_message>
ODYM-RECC v2.4 is running through with mass balance kept.
</commit_message>
<xml_diff>
--- a/RECC_Config_V2_3.xlsx
+++ b/RECC_Config_V2_3.xlsx
@@ -48222,7 +48222,7 @@
       </c>
       <c r="D151" s="93" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
@@ -48245,7 +48245,7 @@
       </c>
       <c r="D152" s="93" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
@@ -48268,7 +48268,7 @@
       </c>
       <c r="D153" s="93" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E153" s="55" t="inlineStr">
@@ -48375,7 +48375,7 @@
       </c>
       <c r="D157" s="93" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
@@ -48421,7 +48421,7 @@
       </c>
       <c r="D159" s="93" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E159" s="55" t="inlineStr">
@@ -48444,7 +48444,7 @@
       </c>
       <c r="D160" s="93" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E160" s="55" t="inlineStr">

</xml_diff>